<commit_message>
Updates in the config files
</commit_message>
<xml_diff>
--- a/Configurations/Config_quick_snap.xlsx
+++ b/Configurations/Config_quick_snap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Edureka\Hadoop Admin\Rahul\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Edureka\Hadoop Admin\Rahul\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -73,9 +73,6 @@
     <t>SNN Dir</t>
   </si>
   <si>
-    <t>DN Dir</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -92,6 +89,10 @@
   </si>
   <si>
     <t>JT URI and Max Mappers/Reducers</t>
+  </si>
+  <si>
+    <t>DN Dir
+Replication Factor</t>
   </si>
 </sst>
 </file>
@@ -459,7 +460,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +469,7 @@
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -585,15 +586,15 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6" s="2" t="s">
-        <v>15</v>
+      <c r="I6" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -615,23 +616,23 @@
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -653,23 +654,23 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -691,23 +692,23 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ansible commands to modify hadoop configs
</commit_message>
<xml_diff>
--- a/Configurations/Config_quick_snap.xlsx
+++ b/Configurations/Config_quick_snap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>NN</t>
   </si>
@@ -92,6 +92,10 @@
   </si>
   <si>
     <t>DN Dir
+Replication Factor</t>
+  </si>
+  <si>
+    <t>NA
 Replication Factor</t>
   </si>
 </sst>
@@ -460,7 +464,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +472,7 @@
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -585,8 +589,8 @@
         <v>14</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>15</v>
+      <c r="G6" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="3" t="s">

</xml_diff>

<commit_message>
modified configs in hdpv1
</commit_message>
<xml_diff>
--- a/Configurations/Config_quick_snap.xlsx
+++ b/Configurations/Config_quick_snap.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8265"/>
   </bookViews>
   <sheets>
-    <sheet name="Config" sheetId="1" r:id="rId1"/>
+    <sheet name="Configv1" sheetId="1" r:id="rId1"/>
     <sheet name="Tasks" sheetId="4" r:id="rId2"/>
     <sheet name="Tools" sheetId="2" r:id="rId3"/>
     <sheet name="To Be checked" sheetId="3" r:id="rId4"/>
@@ -80,17 +80,6 @@
     <t>TT Hostnames</t>
   </si>
   <si>
-    <t>JT URI and Max Mappers/Reducers</t>
-  </si>
-  <si>
-    <t>DN Dir
-Replication Factor</t>
-  </si>
-  <si>
-    <t>NA
-Replication Factor</t>
-  </si>
-  <si>
     <t>navigator cloudera</t>
   </si>
   <si>
@@ -115,16 +104,29 @@
 dfs.secondary.http.address</t>
   </si>
   <si>
+    <t>JT URI
+mapred.hosts.exclude
+mapred.hosts
+mapred.map.tasks.maximum
+mapred.reduce.tasks.maximum</t>
+  </si>
+  <si>
+    <t>JT URI</t>
+  </si>
+  <si>
     <t>NN Dir
 Block size
-Replication Factor
+dfs.replication
 dfs.hosts.exclude
 dfs.hosts</t>
   </si>
   <si>
-    <t>JT URI
-mapred.hosts.exclude
-mapred.hosts</t>
+    <t>NA
+dfs.replication</t>
+  </si>
+  <si>
+    <t>DN Dir
+dfs.replication</t>
   </si>
 </sst>
 </file>
@@ -492,15 +494,15 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="56.28515625" customWidth="1"/>
-    <col min="7" max="7" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -610,19 +612,19 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
@@ -642,7 +644,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -656,7 +658,7 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
@@ -664,7 +666,7 @@
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -767,7 +769,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -790,15 +792,15 @@
   <sheetData>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -818,7 +820,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>